<commit_message>
Start looking at my personal datasets for opporunities
</commit_message>
<xml_diff>
--- a/SWD_EX43.xlsx
+++ b/SWD_EX43.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{354A680F-05FC-43B9-9C71-8209AD5B1E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C523B70-1FC3-4535-A818-F4342E75A062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
+    <workbookView xWindow="8064" yWindow="1620" windowWidth="11592" windowHeight="7944" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>FROM:</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>Problem Statement</t>
+  </si>
+  <si>
+    <t>Internal Discussion</t>
+  </si>
+  <si>
+    <t>I need to find historical projections that compare to actual performance.</t>
+  </si>
+  <si>
+    <t>Some of my battery work may support this.</t>
+  </si>
+  <si>
+    <t>Compare simple model to ODE</t>
   </si>
 </sst>
 </file>
@@ -177,12 +189,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="9"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="9" applyFont="1"/>
     <xf numFmtId="15" fontId="1" fillId="4" borderId="0" xfId="9" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comment" xfId="7" xr:uid="{763C255E-5D87-466E-95B0-D699BCBDC27A}"/>
@@ -443,10 +456,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE64C3D-CB93-427A-A3A9-B177BAA3DAB9}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -476,14 +489,34 @@
       <c r="B3" s="4"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Starting to look at the SWD May challenge problem. The ODE battery solution is a possible one.
</commit_message>
<xml_diff>
--- a/SWD_EX43.xlsx
+++ b/SWD_EX43.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C523B70-1FC3-4535-A818-F4342E75A062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E05EBDB-FCA6-40CB-ADFE-373C3563B284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8064" yWindow="1620" windowWidth="11592" windowHeight="7944" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
+    <workbookView xWindow="24" yWindow="60" windowWidth="11844" windowHeight="7944" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>FROM:</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Compare simple model to ODE</t>
+  </si>
+  <si>
+    <t>This would be a straight line versus a curve.</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE64C3D-CB93-427A-A3A9-B177BAA3DAB9}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -519,6 +522,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Considering other historical predictions.
</commit_message>
<xml_diff>
--- a/SWD_EX43.xlsx
+++ b/SWD_EX43.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E05EBDB-FCA6-40CB-ADFE-373C3563B284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0901CEF-2CE3-4184-8258-2EC303E3C13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="60" windowWidth="11844" windowHeight="7944" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
+    <workbookView xWindow="3000" yWindow="2580" windowWidth="21600" windowHeight="11400" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>FROM:</t>
   </si>
@@ -67,6 +72,9 @@
   </si>
   <si>
     <t>This would be a straight line versus a curve.</t>
+  </si>
+  <si>
+    <t>I need some other alternatives. I could use some other circuit characteristics. Rise time? Power? Predicted operating time still seems like a good one though.</t>
   </si>
 </sst>
 </file>
@@ -459,15 +467,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE64C3D-CB93-427A-A3A9-B177BAA3DAB9}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +484,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -485,46 +493,51 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Old computer fired up. Let's see if this works.
</commit_message>
<xml_diff>
--- a/SWD_EX43.xlsx
+++ b/SWD_EX43.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E05EBDB-FCA6-40CB-ADFE-373C3563B284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0901CEF-2CE3-4184-8258-2EC303E3C13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="60" windowWidth="11844" windowHeight="7944" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
+    <workbookView xWindow="3000" yWindow="2580" windowWidth="21600" windowHeight="11400" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>FROM:</t>
   </si>
@@ -67,6 +72,9 @@
   </si>
   <si>
     <t>This would be a straight line versus a curve.</t>
+  </si>
+  <si>
+    <t>I need some other alternatives. I could use some other circuit characteristics. Rise time? Power? Predicted operating time still seems like a good one though.</t>
   </si>
 </sst>
 </file>
@@ -459,15 +467,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE64C3D-CB93-427A-A3A9-B177BAA3DAB9}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +484,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -485,46 +493,51 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I am thinking the nonlinearity may be better handled in Mathcad
</commit_message>
<xml_diff>
--- a/SWD_EX43.xlsx
+++ b/SWD_EX43.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0901CEF-2CE3-4184-8258-2EC303E3C13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898DB78D-600C-448F-A382-642E15FE546F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="2580" windowWidth="21600" windowHeight="11400" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11400" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>FROM:</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>I need some other alternatives. I could use some other circuit characteristics. Rise time? Power? Predicted operating time still seems like a good one though.</t>
+  </si>
+  <si>
+    <t>I may want to try this in Mathcad first.</t>
   </si>
 </sst>
 </file>
@@ -467,10 +470,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE64C3D-CB93-427A-A3A9-B177BAA3DAB9}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -540,6 +543,11 @@
         <v>12</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Still having trouble getting started
</commit_message>
<xml_diff>
--- a/SWD_EX43.xlsx
+++ b/SWD_EX43.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898DB78D-600C-448F-A382-642E15FE546F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A45F45-47FA-484C-B291-46668ADA595B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11400" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11400" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>FROM:</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>I may want to try this in Mathcad first.</t>
+  </si>
+  <si>
+    <t>I am still not seeing April in the solutions.</t>
   </si>
 </sst>
 </file>
@@ -470,10 +473,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE64C3D-CB93-427A-A3A9-B177BAA3DAB9}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -548,6 +551,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
More comment on graphic format
</commit_message>
<xml_diff>
--- a/SWD_EX43.xlsx
+++ b/SWD_EX43.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A45F45-47FA-484C-B291-46668ADA595B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434FC188-C2EF-4614-BE18-9A20830F8092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11400" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11400" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>FROM:</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>I am still not seeing April in the solutions.</t>
+  </si>
+  <si>
+    <t>Could I try projections on ice out dates?</t>
   </si>
 </sst>
 </file>
@@ -473,10 +476,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE64C3D-CB93-427A-A3A9-B177BAA3DAB9}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -556,6 +559,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>